<commit_message>
Submitting changes applied to backstage scenarios.
</commit_message>
<xml_diff>
--- a/Data Files/GoPro_UI_Verification.xlsx
+++ b/Data Files/GoPro_UI_Verification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\Data-Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AutoTest_1\git\PINS_ODT_NEW_TEST\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F81477F-30BE-4B8E-A35F-2DCD604135A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8311FCA3-62CC-4539-B698-FA218CB819E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{54CE332F-CBA2-47CB-8B23-5DC5DAF8AFDA}"/>
   </bookViews>
@@ -79,17 +79,18 @@
     <t>Appeal Decision Cover Letter</t>
   </si>
   <si>
+    <t>Appeal Decision</t>
+  </si>
+  <si>
     <t xml:space="preserve">                                
                                 ARSV
                                 ASV
                                 USV
                                 VSV
                                 NSV
+                                USV+
                                 Hearing
                             </t>
-  </si>
-  <si>
-    <t>Appeal Decision</t>
   </si>
 </sst>
 </file>
@@ -447,7 +448,7 @@
   <dimension ref="A1:A76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -475,9 +476,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
@@ -527,7 +528,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
New Test added for Picaso login checks.
</commit_message>
<xml_diff>
--- a/Data Files/GoPro_UI_Verification.xlsx
+++ b/Data Files/GoPro_UI_Verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AutoTest_1\git\PINS_ODT_NEW_TEST\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8311FCA3-62CC-4539-B698-FA218CB819E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6331403D-299F-467D-A400-225C68EC399C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{54CE332F-CBA2-47CB-8B23-5DC5DAF8AFDA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Verifications </t>
   </si>
@@ -91,6 +91,9 @@
                                 USV+
                                 Hearing
                             </t>
+  </si>
+  <si>
+    <t>Invalid credentials. Try again.</t>
   </si>
 </sst>
 </file>
@@ -447,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192F818B-9F99-4506-AB8C-E6CF706CA6D3}">
   <dimension ref="A1:A76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -531,6 +534,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
     </row>

</xml_diff>